<commit_message>
[FIX] z0bug_odoo with python3
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/miscellaneous.xlsx
+++ b/z0bug_odoo/data/miscellaneous.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t xml:space="preserve">True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base.group_no_one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sale.group_delivery_invoice_address</t>
   </si>
 </sst>
 </file>
@@ -65,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,11 +92,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,12 +136,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -165,16 +162,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.81"/>
   </cols>
   <sheetData>
@@ -194,7 +191,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -224,6 +221,28 @@
         <v>10</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>